<commit_message>
Added Conflict and fragile country grouping from World Bank 2024
</commit_message>
<xml_diff>
--- a/Reference/UN M49 code.xlsx
+++ b/Reference/UN M49 code.xlsx
@@ -4651,8 +4651,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087FEDB81126C72489E896866974B8D20" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6b39e01ff3b0124afd8f1865415e282d">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="583c1edc-5697-44bf-8915-bcc017c6315e" xmlns:ns3="683382e9-ecfe-41ed-b4c8-69ea71b11d74" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a9d930256b85b31bb793601de56bd166" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087FEDB81126C72489E896866974B8D20" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c26d39bc55fc011234c285d3e63a6473">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="583c1edc-5697-44bf-8915-bcc017c6315e" xmlns:ns3="683382e9-ecfe-41ed-b4c8-69ea71b11d74" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="94bd697067cf947214e38e2284831c70" ns2:_="" ns3:_="">
     <xsd:import namespace="583c1edc-5697-44bf-8915-bcc017c6315e"/>
     <xsd:import namespace="683382e9-ecfe-41ed-b4c8-69ea71b11d74"/>
     <xsd:element name="properties">
@@ -4665,6 +4665,8 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -4681,6 +4683,16 @@
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="12" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="13" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
@@ -4831,7 +4843,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB292AF2-8F15-4EA7-922C-0EF0802E829A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8A02215-10CC-49FE-9062-64B034825EAF}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>